<commit_message>
fixed: this.qtyIndex -> this.qtyModIndex
</commit_message>
<xml_diff>
--- a/prodID/prodID.xlsx
+++ b/prodID/prodID.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\nodejs\csrz\prodID\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11700"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>品番</t>
   </si>
@@ -24,9 +29,6 @@
     <t>TPMS传感器编号</t>
   </si>
   <si>
-    <t xml:space="preserve">4E5DR </t>
-  </si>
-  <si>
     <t>4250F557</t>
   </si>
   <si>
@@ -58,9 +60,6 @@
   </si>
   <si>
     <t>4250F293</t>
-  </si>
-  <si>
-    <t>GT</t>
   </si>
   <si>
     <t>TPMS传感器型号</t>
@@ -106,8 +105,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,9 +143,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -154,23 +156,94 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -205,7 +278,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,9 +310,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,6 +345,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,147 +521,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CBE124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.375" customWidth="1"/>
-    <col min="2" max="2" width="15.375" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="BX1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:76">
-      <c r="A2" t="s">
+      <c r="B2" s="1">
         <v>3</v>
       </c>
-      <c r="B2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:76">
-      <c r="A3" t="s">
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:76">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:76">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:76">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:76">
-      <c r="A7" t="s">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:76">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:76">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:76">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:76">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:76">
-      <c r="A12" t="s">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:76">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:76">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>-1</v>
-      </c>
-    </row>
-    <row r="124" spans="2085:2085">
-      <c r="CBE124" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -596,48 +663,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -647,33 +714,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="32.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed receive repeated complete message. added send VIN to TPMS
</commit_message>
<xml_diff>
--- a/prodID/prodID.xlsx
+++ b/prodID/prodID.xlsx
@@ -117,6 +117,7 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -525,7 +526,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -653,7 +654,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug: printCSV took wrong sheet name, should be last sheetname not next
</commit_message>
<xml_diff>
--- a/prodID/prodID.xlsx
+++ b/prodID/prodID.xlsx
@@ -82,14 +82,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>C:/nodejs/print</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:/nodejs/tempdata/result.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3110009ADU1300C10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -99,6 +91,14 @@
   </si>
   <si>
     <t>轮胎数量调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:/source/nodejs/tempdata/result.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:/source/nodejs/print</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -581,7 +581,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -719,13 +719,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="32.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -738,10 +738,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>